<commit_message>
code optimised and cleaned
</commit_message>
<xml_diff>
--- a/backend/cleansed_files/cleansed_File_008.xlsx
+++ b/backend/cleansed_files/cleansed_File_008.xlsx
@@ -867,7 +867,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>HT-98976-AL</t>
+          <t>HT-98976-[REDACTED]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>HT-98976-AL</t>
+          <t>HT-98976-[REDACTED]</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">

</xml_diff>